<commit_message>
se quito parte del mensje
</commit_message>
<xml_diff>
--- a/usuarios.xlsx
+++ b/usuarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria.yeguez\Documents\GitHub\phishing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB60D256-06E6-4D2B-83FF-9730FB122E75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD45150E-DFF2-4997-9E98-53E4B89D7C1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>nombres</t>
   </si>
@@ -76,13 +76,25 @@
   </si>
   <si>
     <t>JF3</t>
+  </si>
+  <si>
+    <t>correo</t>
+  </si>
+  <si>
+    <t>mariavyeguezp@gmail.com</t>
+  </si>
+  <si>
+    <t>r.gzlobos@gmail.com</t>
+  </si>
+  <si>
+    <t>ma.yeguez@duocuc.cl</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,6 +104,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -114,13 +134,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -399,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -412,9 +435,10 @@
     <col min="4" max="4" width="26.36328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31.1796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -433,8 +457,11 @@
       <c r="F1" t="s">
         <v>7</v>
       </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -453,8 +480,11 @@
       <c r="F2" t="s">
         <v>12</v>
       </c>
+      <c r="G2" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -473,8 +503,11 @@
       <c r="F3" t="s">
         <v>5</v>
       </c>
+      <c r="G3" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -492,10 +525,18 @@
       </c>
       <c r="F4" t="s">
         <v>12</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{2EAC21AD-C2FF-4176-8E95-E409E4D15DF7}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{481B5B0C-E85C-4F77-9336-42EDCC8A437C}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{6335D8D3-ACDF-4C64-8B28-17B0709E3C82}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>